<commit_message>
se suben escenarios de excel "contabilidad electronica"
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_003_AdvantageTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_003_AdvantageTest.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A23E44-50AB-41D1-854F-8981AD8613B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92A7BF8-1005-4E10-A6B2-1E902272CF2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>